<commit_message>
minor update to atttributable breakdown figure
</commit_message>
<xml_diff>
--- a/final_combined_2methods_wide_ff.xlsx
+++ b/final_combined_2methods_wide_ff.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JohnMatthew/Downloads/Thorne_15_codefigurestats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JohnMatthew/Downloads/Thorne_15/FaIR_fut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75DEAE30-8CF3-BD4B-BF7D-8788CC9B005C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BB3260A-2D9E-9D4D-899C-E61AD7F6BC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17080" yWindow="3160" windowWidth="26840" windowHeight="15940" xr2:uid="{C5EFB806-CC49-FF45-A9BF-684F2EA9307C}"/>
+    <workbookView xWindow="7580" yWindow="5220" windowWidth="26840" windowHeight="15940" xr2:uid="{C5EFB806-CC49-FF45-A9BF-684F2EA9307C}"/>
   </bookViews>
   <sheets>
     <sheet name="final_combined_2methods_wide_ff" sheetId="1" r:id="rId1"/>
@@ -140,9 +140,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -622,11 +622,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -693,153 +696,153 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="final_combined_8methods_wide_ff"/>
+      <sheetName val="final_combined_16methods_wide_f"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="A3" t="str">
+        <row r="2">
+          <cell r="A2" t="str">
             <v>fut_ESM1-2-LR_SSP126_constVolc</v>
           </cell>
-          <cell r="C3">
-            <v>0.22308304915471799</v>
-          </cell>
-          <cell r="D3">
-            <v>0.424566875229338</v>
-          </cell>
-          <cell r="E3">
-            <v>0.79550180909741797</v>
-          </cell>
-          <cell r="F3">
-            <v>0.52683259573418595</v>
-          </cell>
-          <cell r="G3">
-            <v>0</v>
-          </cell>
-          <cell r="H3">
-            <v>1.4</v>
-          </cell>
-          <cell r="I3">
-            <v>3.40471680358857E-2</v>
-          </cell>
-          <cell r="J3">
-            <v>3.3809669212986698E-2</v>
+          <cell r="C2">
+            <v>0.23423231205582501</v>
+          </cell>
+          <cell r="D2">
+            <v>0.44301513220746003</v>
+          </cell>
+          <cell r="E2">
+            <v>0.80477747916472697</v>
+          </cell>
+          <cell r="F2">
+            <v>0.46624181380279101</v>
+          </cell>
+          <cell r="G2">
+            <v>0.49304442107483998</v>
+          </cell>
+          <cell r="H2">
+            <v>1.22</v>
+          </cell>
+          <cell r="I2">
+            <v>3.4209966316283001E-2</v>
+          </cell>
+          <cell r="J2">
+            <v>3.3170670153985497E-2</v>
           </cell>
         </row>
-        <row r="5">
-          <cell r="A5" t="str">
+        <row r="4">
+          <cell r="A4" t="str">
             <v>fut_ESM1-2-LR_SSP245_constVolc</v>
           </cell>
-          <cell r="C5">
-            <v>0.569109432515022</v>
-          </cell>
-          <cell r="D5">
-            <v>0.86701193830489198</v>
-          </cell>
-          <cell r="E5">
-            <v>0.99221729758710098</v>
-          </cell>
-          <cell r="F5">
-            <v>0.40258795692067401</v>
-          </cell>
-          <cell r="G5">
-            <v>0</v>
-          </cell>
-          <cell r="H5">
+          <cell r="C4">
+            <v>0.54526216461403398</v>
+          </cell>
+          <cell r="D4">
+            <v>0.85151612528392695</v>
+          </cell>
+          <cell r="E4">
+            <v>0.98769878415374102</v>
+          </cell>
+          <cell r="F4">
+            <v>0.34391488294497302</v>
+          </cell>
+          <cell r="G4">
+            <v>0.33005863001684399</v>
+          </cell>
+          <cell r="H4">
+            <v>1.02</v>
+          </cell>
+          <cell r="I4">
+            <v>3.1604406760897701E-2</v>
+          </cell>
+          <cell r="J4">
+            <v>2.94731342330086E-2</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>fut_ESM1-2-LR_SSP370_constVolc</v>
+          </cell>
+          <cell r="C6">
+            <v>0.58820103523420497</v>
+          </cell>
+          <cell r="D6">
+            <v>0.882503084666731</v>
+          </cell>
+          <cell r="E6">
+            <v>0.99999998110849297</v>
+          </cell>
+          <cell r="F6">
+            <v>0.25605969664375</v>
+          </cell>
+          <cell r="G6">
+            <v>0.18398203276660599</v>
+          </cell>
+          <cell r="H6">
             <v>1</v>
           </cell>
-          <cell r="I5">
-            <v>3.14806872842225E-2</v>
-          </cell>
-          <cell r="J5">
-            <v>3.01916331118126E-2</v>
+          <cell r="I6">
+            <v>3.2646386575724898E-2</v>
+          </cell>
+          <cell r="J6">
+            <v>2.8700340830130601E-2</v>
           </cell>
         </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>fut_ESM1-2-LR_SSP370_constVolc</v>
-          </cell>
-          <cell r="C7">
-            <v>0.60784617948213104</v>
-          </cell>
-          <cell r="D7">
-            <v>0.89568249198837102</v>
-          </cell>
-          <cell r="E7">
-            <v>0.99999998981716498</v>
-          </cell>
-          <cell r="F7">
-            <v>0.30125529255462702</v>
-          </cell>
-          <cell r="G7">
-            <v>0</v>
-          </cell>
-          <cell r="H7">
-            <v>1.06</v>
-          </cell>
-          <cell r="I7">
-            <v>3.1189349837246302E-2</v>
-          </cell>
-          <cell r="J7">
-            <v>2.8401842232407101E-2</v>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>fut_NorESM_RCP45_Volc</v>
+          </cell>
+          <cell r="C8">
+            <v>0.31504677447179003</v>
+          </cell>
+          <cell r="D8">
+            <v>0.57232123229446896</v>
+          </cell>
+          <cell r="E8">
+            <v>0.89159107765915202</v>
+          </cell>
+          <cell r="F8">
+            <v>0.65038981916972405</v>
+          </cell>
+          <cell r="G8">
+            <v>0.69969231489820405</v>
+          </cell>
+          <cell r="H8">
+            <v>1.1000000000000001</v>
+          </cell>
+          <cell r="I8">
+            <v>4.9608096699926101E-2</v>
+          </cell>
+          <cell r="J8">
+            <v>5.1449692451564499E-2</v>
           </cell>
         </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>fut_NorESM_RCP45_Volc</v>
-          </cell>
-          <cell r="C9">
-            <v>0.33924081974388598</v>
-          </cell>
-          <cell r="D9">
-            <v>0.61175353856367198</v>
-          </cell>
-          <cell r="E9">
-            <v>0.92475270821782396</v>
-          </cell>
-          <cell r="F9">
-            <v>0.63527200384498705</v>
-          </cell>
-          <cell r="G9">
-            <v>0</v>
-          </cell>
-          <cell r="H9">
-            <v>1.06666666666666</v>
-          </cell>
-          <cell r="I9">
-            <v>4.5672518021823302E-2</v>
-          </cell>
-          <cell r="J9">
-            <v>4.7148170683740498E-2</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
+        <row r="10">
+          <cell r="A10" t="str">
             <v>fut_NorESM_RCP45_VolcConst</v>
           </cell>
-          <cell r="C11">
-            <v>0.582823059441401</v>
-          </cell>
-          <cell r="D11">
-            <v>0.88205120151754801</v>
-          </cell>
-          <cell r="E11">
-            <v>0.99999399718521598</v>
-          </cell>
-          <cell r="F11">
-            <v>0.42914306835327898</v>
-          </cell>
-          <cell r="G11">
-            <v>0</v>
-          </cell>
-          <cell r="H11">
+          <cell r="C10">
+            <v>0.60445409265483296</v>
+          </cell>
+          <cell r="D10">
+            <v>0.91644379909259599</v>
+          </cell>
+          <cell r="E10">
+            <v>0.99999999918240301</v>
+          </cell>
+          <cell r="F10">
+            <v>0.39538783081048301</v>
+          </cell>
+          <cell r="G10">
+            <v>0.42024078216599597</v>
+          </cell>
+          <cell r="H10">
             <v>1.0166666666666599</v>
           </cell>
-          <cell r="I11">
-            <v>2.69319364673281E-2</v>
-          </cell>
-          <cell r="J11">
-            <v>2.6904618104796E-2</v>
+          <cell r="I10">
+            <v>2.8010350719259801E-2</v>
+          </cell>
+          <cell r="J10">
+            <v>2.7966801098772701E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -855,153 +858,153 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="final_combined_16methods_wide_f"/>
+      <sheetName val="final_combined_7methods_wide_ff"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2" t="str">
+        <row r="3">
+          <cell r="A3" t="str">
             <v>fut_ESM1-2-LR_SSP126_constVolc</v>
           </cell>
-          <cell r="C2">
-            <v>0.23423231205582501</v>
-          </cell>
-          <cell r="D2">
-            <v>0.44301513220746003</v>
-          </cell>
-          <cell r="E2">
-            <v>0.80477747916472697</v>
-          </cell>
-          <cell r="F2">
-            <v>0.46624181380279101</v>
-          </cell>
-          <cell r="G2">
-            <v>0.49304442107483998</v>
-          </cell>
-          <cell r="H2">
-            <v>1.22</v>
-          </cell>
-          <cell r="I2">
-            <v>3.4209966316283001E-2</v>
-          </cell>
-          <cell r="J2">
-            <v>3.3170670153985497E-2</v>
+          <cell r="C3">
+            <v>0.20598707423877799</v>
+          </cell>
+          <cell r="D3">
+            <v>0.39125892210348001</v>
+          </cell>
+          <cell r="E3">
+            <v>0.75460221525915105</v>
+          </cell>
+          <cell r="F3">
+            <v>0.56475621844510304</v>
+          </cell>
+          <cell r="G3">
+            <v>0</v>
+          </cell>
+          <cell r="H3">
+            <v>1.42</v>
+          </cell>
+          <cell r="I3">
+            <v>3.52982195739854E-2</v>
+          </cell>
+          <cell r="J3">
+            <v>3.4435063627015101E-2</v>
           </cell>
         </row>
-        <row r="4">
-          <cell r="A4" t="str">
+        <row r="5">
+          <cell r="A5" t="str">
             <v>fut_ESM1-2-LR_SSP245_constVolc</v>
           </cell>
-          <cell r="C4">
-            <v>0.54526216461403398</v>
-          </cell>
-          <cell r="D4">
-            <v>0.85151612528392695</v>
-          </cell>
-          <cell r="E4">
-            <v>0.98769878415374102</v>
-          </cell>
-          <cell r="F4">
-            <v>0.34391488294497302</v>
-          </cell>
-          <cell r="G4">
-            <v>0.33005863001684399</v>
-          </cell>
-          <cell r="H4">
-            <v>1.02</v>
-          </cell>
-          <cell r="I4">
-            <v>3.1604406760897701E-2</v>
-          </cell>
-          <cell r="J4">
-            <v>2.94731342330086E-2</v>
+          <cell r="C5">
+            <v>0.54537720214768104</v>
+          </cell>
+          <cell r="D5">
+            <v>0.82936652432745805</v>
+          </cell>
+          <cell r="E5">
+            <v>0.98938446493499099</v>
+          </cell>
+          <cell r="F5">
+            <v>0.47702824636535701</v>
+          </cell>
+          <cell r="G5">
+            <v>0</v>
+          </cell>
+          <cell r="H5">
+            <v>1.04</v>
+          </cell>
+          <cell r="I5">
+            <v>3.20702585058706E-2</v>
+          </cell>
+          <cell r="J5">
+            <v>2.9932675985723699E-2</v>
           </cell>
         </row>
-        <row r="6">
-          <cell r="A6" t="str">
+        <row r="7">
+          <cell r="A7" t="str">
             <v>fut_ESM1-2-LR_SSP370_constVolc</v>
           </cell>
-          <cell r="C6">
-            <v>0.58820103523420497</v>
-          </cell>
-          <cell r="D6">
-            <v>0.882503084666731</v>
-          </cell>
-          <cell r="E6">
-            <v>0.99999998110849297</v>
-          </cell>
-          <cell r="F6">
-            <v>0.25605969664375</v>
-          </cell>
-          <cell r="G6">
-            <v>0.18398203276660599</v>
-          </cell>
-          <cell r="H6">
+          <cell r="C7">
+            <v>0.54377625772486804</v>
+          </cell>
+          <cell r="D7">
+            <v>0.85010427686262902</v>
+          </cell>
+          <cell r="E7">
+            <v>0.99999241359801805</v>
+          </cell>
+          <cell r="F7">
+            <v>0.35240261158414299</v>
+          </cell>
+          <cell r="G7">
+            <v>0</v>
+          </cell>
+          <cell r="H7">
+            <v>1.08</v>
+          </cell>
+          <cell r="I7">
+            <v>3.6908175403974099E-2</v>
+          </cell>
+          <cell r="J7">
+            <v>3.3497276994360899E-2</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>fut_NorESM_RCP45_Volc</v>
+          </cell>
+          <cell r="C9">
+            <v>0.29728047786762701</v>
+          </cell>
+          <cell r="D9">
+            <v>0.54511819223838698</v>
+          </cell>
+          <cell r="E9">
+            <v>0.87959810607169198</v>
+          </cell>
+          <cell r="F9">
+            <v>0.75713434312233396</v>
+          </cell>
+          <cell r="G9">
+            <v>0</v>
+          </cell>
+          <cell r="H9">
+            <v>1.11666666666666</v>
+          </cell>
+          <cell r="I9">
+            <v>4.9593159564462398E-2</v>
+          </cell>
+          <cell r="J9">
+            <v>5.1204322773566999E-2</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>fut_NorESM_RCP45_VolcConst</v>
+          </cell>
+          <cell r="C11">
+            <v>0.54102601968391995</v>
+          </cell>
+          <cell r="D11">
+            <v>0.86734724522561701</v>
+          </cell>
+          <cell r="E11">
+            <v>0.99999820550391105</v>
+          </cell>
+          <cell r="F11">
+            <v>0.588634202813348</v>
+          </cell>
+          <cell r="G11">
+            <v>0</v>
+          </cell>
+          <cell r="H11">
             <v>1</v>
           </cell>
-          <cell r="I6">
-            <v>3.2646386575724898E-2</v>
-          </cell>
-          <cell r="J6">
-            <v>2.8700340830130601E-2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>fut_NorESM_RCP45_Volc</v>
-          </cell>
-          <cell r="C8">
-            <v>0.31504677447179003</v>
-          </cell>
-          <cell r="D8">
-            <v>0.57232123229446896</v>
-          </cell>
-          <cell r="E8">
-            <v>0.89159107765915202</v>
-          </cell>
-          <cell r="F8">
-            <v>0.65038981916972405</v>
-          </cell>
-          <cell r="G8">
-            <v>0.69969231489820405</v>
-          </cell>
-          <cell r="H8">
-            <v>1.1000000000000001</v>
-          </cell>
-          <cell r="I8">
-            <v>4.9608096699926101E-2</v>
-          </cell>
-          <cell r="J8">
-            <v>5.1449692451564499E-2</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>fut_NorESM_RCP45_VolcConst</v>
-          </cell>
-          <cell r="C10">
-            <v>0.60445409265483296</v>
-          </cell>
-          <cell r="D10">
-            <v>0.91644379909259599</v>
-          </cell>
-          <cell r="E10">
-            <v>0.99999999918240301</v>
-          </cell>
-          <cell r="F10">
-            <v>0.39538783081048301</v>
-          </cell>
-          <cell r="G10">
-            <v>0.42024078216599597</v>
-          </cell>
-          <cell r="H10">
-            <v>1.0166666666666599</v>
-          </cell>
-          <cell r="I10">
-            <v>2.8010350719259801E-2</v>
-          </cell>
-          <cell r="J10">
-            <v>2.7966801098772701E-2</v>
+          <cell r="I11">
+            <v>2.9942905637516601E-2</v>
+          </cell>
+          <cell r="J11">
+            <v>3.0024013511340601E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -1329,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB62F910-86A1-8841-8AC9-30F3B8F67705}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,28 +1382,28 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>0.193323599140513</v>
+        <v>0.21161932405351599</v>
       </c>
       <c r="D2">
-        <v>0.380216728418869</v>
+        <v>0.40396595365675098</v>
       </c>
       <c r="E2">
-        <v>0.78584092298366603</v>
+        <v>0.76865427585143098</v>
       </c>
       <c r="F2">
-        <v>0.59962577107472603</v>
+        <v>0.63734650833749396</v>
       </c>
       <c r="G2">
-        <v>0.62717374477799903</v>
+        <v>0.52549062434882099</v>
       </c>
       <c r="H2">
-        <v>1.52</v>
+        <v>1.54</v>
       </c>
       <c r="I2">
-        <v>3.9122765985414802E-2</v>
+        <v>4.14550484967314E-2</v>
       </c>
       <c r="J2">
-        <v>3.9793504476862397E-2</v>
+        <v>3.5818757452349699E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1420,19 +1423,19 @@
         <v>0.67738862149364099</v>
       </c>
       <c r="F3">
-        <v>0.71566361962981095</v>
+        <v>0.72312962730627905</v>
       </c>
       <c r="G3">
-        <v>0.64250108122296601</v>
+        <v>0.65262018332211302</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>4.8024178941443202E-2</v>
+        <v>4.7924826086253897E-2</v>
       </c>
       <c r="J3">
-        <v>3.96099663956316E-2</v>
+        <v>3.9585073275757901E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1443,28 +1446,28 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>0.53135273482905598</v>
+        <v>0.50974682042109598</v>
       </c>
       <c r="D4">
-        <v>0.82636970138093202</v>
+        <v>0.80996193536411498</v>
       </c>
       <c r="E4">
-        <v>0.99079631936799195</v>
+        <v>0.98746274665149802</v>
       </c>
       <c r="F4">
-        <v>0.55943310164726401</v>
+        <v>0.56415571141182597</v>
       </c>
       <c r="G4">
-        <v>0.58678766020784501</v>
+        <v>0.39092663554097901</v>
       </c>
       <c r="H4">
         <v>1.02</v>
       </c>
       <c r="I4">
-        <v>3.9053609917750497E-2</v>
+        <v>3.9619484294593298E-2</v>
       </c>
       <c r="J4">
-        <v>4.01043089335959E-2</v>
+        <v>3.2487978546580497E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1484,19 +1487,19 @@
         <v>0.92550530731992098</v>
       </c>
       <c r="F5">
-        <v>0.70551346522369296</v>
+        <v>0.71242307999963705</v>
       </c>
       <c r="G5">
-        <v>0.60169079932651703</v>
+        <v>0.61013150635878699</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>5.1673175527618499E-2</v>
+        <v>5.14577615073573E-2</v>
       </c>
       <c r="J5">
-        <v>4.0134199225987002E-2</v>
+        <v>3.9952145868938999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1507,28 +1510,28 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>0.576123416097439</v>
+        <v>0.64167468205339295</v>
       </c>
       <c r="D6">
-        <v>0.84515713805507198</v>
+        <v>0.92134192098814205</v>
       </c>
       <c r="E6">
-        <v>0.99999825056773195</v>
+        <v>0.99999999992211497</v>
       </c>
       <c r="F6">
-        <v>0.66091742730965497</v>
+        <v>0.58257242065806303</v>
       </c>
       <c r="G6">
-        <v>0.67416000173234703</v>
+        <v>0.36471938323216702</v>
       </c>
       <c r="H6">
         <v>1.06</v>
       </c>
       <c r="I6">
-        <v>3.5884994681368902E-2</v>
+        <v>3.9146185155741801E-2</v>
       </c>
       <c r="J6">
-        <v>3.5317593409777699E-2</v>
+        <v>2.9479803361305599E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1548,19 +1551,19 @@
         <v>0.82410366011376901</v>
       </c>
       <c r="F7">
-        <v>0.74998847518916401</v>
+        <v>0.75525220045584596</v>
       </c>
       <c r="G7">
-        <v>0.64781887558101903</v>
+        <v>0.65528228338484396</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
-        <v>6.8275797525348E-2</v>
+        <v>6.8233767139105395E-2</v>
       </c>
       <c r="J7">
-        <v>5.7196022704550702E-2</v>
+        <v>5.7310887082711301E-2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1571,28 +1574,28 @@
         <v>11</v>
       </c>
       <c r="C8">
-        <v>0.243835969387696</v>
+        <v>0.35316813126645102</v>
       </c>
       <c r="D8">
-        <v>0.47229445778025297</v>
+        <v>0.62991221212830595</v>
       </c>
       <c r="E8">
-        <v>0.88069455042945799</v>
+        <v>0.92104559023504595</v>
       </c>
       <c r="F8">
-        <v>0.78916143656328597</v>
+        <v>0.69470880820399195</v>
       </c>
       <c r="G8">
-        <v>0.88403148247910701</v>
+        <v>0.65259499157233103</v>
       </c>
       <c r="H8">
-        <v>1.06666666666666</v>
+        <v>1.11666666666666</v>
       </c>
       <c r="I8">
-        <v>6.6871679914844107E-2</v>
+        <v>5.9639432635513898E-2</v>
       </c>
       <c r="J8">
-        <v>7.3539784970054894E-2</v>
+        <v>6.0089927606266198E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1635,28 +1638,28 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>0.319788720307984</v>
+        <v>0.49934996162543499</v>
       </c>
       <c r="D10">
-        <v>0.56955446780037</v>
+        <v>0.85184374092964499</v>
       </c>
       <c r="E10">
-        <v>0.96033614214204599</v>
+        <v>0.99999419553518598</v>
       </c>
       <c r="F10">
-        <v>0.71834740073190295</v>
+        <v>0.57230663609077204</v>
       </c>
       <c r="G10">
-        <v>0.77965408123227697</v>
+        <v>0.42470431846740098</v>
       </c>
       <c r="H10">
-        <v>1.0333333333333301</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>4.9759412080330703E-2</v>
+        <v>2.9102690918756099E-2</v>
       </c>
       <c r="J10">
-        <v>5.4092470432414802E-2</v>
+        <v>2.49146921749391E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1741,223 +1744,213 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>[1]final_combined_8methods_wide_ff!A$3</f>
-        <v>fut_ESM1-2-LR_SSP126_constVolc</v>
+        <f>[2]final_combined_7methods_wide_ff!A$7</f>
+        <v>fut_ESM1-2-LR_SSP370_constVolc</v>
       </c>
       <c r="B16" t="str">
         <f>RIGHT(A16,LEN(A16)-4)</f>
-        <v>ESM1-2-LR_SSP126_constVolc</v>
+        <v>ESM1-2-LR_SSP370_constVolc</v>
       </c>
       <c r="C16" s="3">
-        <f>[1]final_combined_8methods_wide_ff!C$3</f>
-        <v>0.22308304915471799</v>
+        <f>[2]final_combined_7methods_wide_ff!C$7</f>
+        <v>0.54377625772486804</v>
       </c>
       <c r="D16" s="3">
-        <f>[1]final_combined_8methods_wide_ff!D$3</f>
-        <v>0.424566875229338</v>
+        <f>[2]final_combined_7methods_wide_ff!D$7</f>
+        <v>0.85010427686262902</v>
       </c>
       <c r="E16" s="3">
-        <f>[1]final_combined_8methods_wide_ff!E$3</f>
-        <v>0.79550180909741797</v>
-      </c>
-      <c r="F16" s="2">
-        <f>[1]final_combined_8methods_wide_ff!F$3</f>
-        <v>0.52683259573418595</v>
-      </c>
-      <c r="G16" s="2">
-        <f>[1]final_combined_8methods_wide_ff!G$3</f>
+        <f>[2]final_combined_7methods_wide_ff!E$7</f>
+        <v>0.99999241359801805</v>
+      </c>
+      <c r="F16" s="6">
+        <f>[2]final_combined_7methods_wide_ff!F$7</f>
+        <v>0.35240261158414299</v>
+      </c>
+      <c r="G16" s="6">
+        <f>[2]final_combined_7methods_wide_ff!G$7</f>
         <v>0</v>
       </c>
-      <c r="H16" s="2">
-        <f>[1]final_combined_8methods_wide_ff!H$3</f>
-        <v>1.4</v>
-      </c>
-      <c r="I16" s="1">
-        <f>[1]final_combined_8methods_wide_ff!I$3</f>
-        <v>3.40471680358857E-2</v>
-      </c>
-      <c r="J16" s="1">
-        <f>[1]final_combined_8methods_wide_ff!J$3</f>
-        <v>3.3809669212986698E-2</v>
+      <c r="H16" s="6">
+        <f>[2]final_combined_7methods_wide_ff!H$7</f>
+        <v>1.08</v>
+      </c>
+      <c r="I16" s="5">
+        <f>[2]final_combined_7methods_wide_ff!I$7</f>
+        <v>3.6908175403974099E-2</v>
+      </c>
+      <c r="J16" s="5">
+        <f>[2]final_combined_7methods_wide_ff!J$7</f>
+        <v>3.3497276994360899E-2</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>[1]final_combined_8methods_wide_ff!A$5</f>
+        <f>[2]final_combined_7methods_wide_ff!A$5</f>
         <v>fut_ESM1-2-LR_SSP245_constVolc</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" ref="B17:B41" si="0">RIGHT(A17,LEN(A17)-4)</f>
+        <f t="shared" ref="B17:B39" si="0">RIGHT(A17,LEN(A17)-4)</f>
         <v>ESM1-2-LR_SSP245_constVolc</v>
       </c>
       <c r="C17" s="3">
-        <f>[1]final_combined_8methods_wide_ff!C$5</f>
-        <v>0.569109432515022</v>
+        <f>[2]final_combined_7methods_wide_ff!C$5</f>
+        <v>0.54537720214768104</v>
       </c>
       <c r="D17" s="3">
-        <f>[1]final_combined_8methods_wide_ff!D$5</f>
-        <v>0.86701193830489198</v>
+        <f>[2]final_combined_7methods_wide_ff!D$5</f>
+        <v>0.82936652432745805</v>
       </c>
       <c r="E17" s="3">
-        <f>[1]final_combined_8methods_wide_ff!E$5</f>
-        <v>0.99221729758710098</v>
-      </c>
-      <c r="F17" s="2">
-        <f>[1]final_combined_8methods_wide_ff!F$5</f>
-        <v>0.40258795692067401</v>
-      </c>
-      <c r="G17" s="2">
-        <f>[1]final_combined_8methods_wide_ff!G$5</f>
+        <f>[2]final_combined_7methods_wide_ff!E$5</f>
+        <v>0.98938446493499099</v>
+      </c>
+      <c r="F17" s="6">
+        <f>[2]final_combined_7methods_wide_ff!F$5</f>
+        <v>0.47702824636535701</v>
+      </c>
+      <c r="G17" s="6">
+        <f>[2]final_combined_7methods_wide_ff!G$5</f>
         <v>0</v>
       </c>
-      <c r="H17" s="2">
-        <f>[1]final_combined_8methods_wide_ff!H$5</f>
-        <v>1</v>
-      </c>
-      <c r="I17" s="1">
-        <f>[1]final_combined_8methods_wide_ff!I$5</f>
-        <v>3.14806872842225E-2</v>
-      </c>
-      <c r="J17" s="1">
-        <f>[1]final_combined_8methods_wide_ff!J$5</f>
-        <v>3.01916331118126E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H17" s="6">
+        <f>[2]final_combined_7methods_wide_ff!H$5</f>
+        <v>1.04</v>
+      </c>
+      <c r="I17" s="5">
+        <f>[2]final_combined_7methods_wide_ff!I$5</f>
+        <v>3.20702585058706E-2</v>
+      </c>
+      <c r="J17" s="5">
+        <f>[2]final_combined_7methods_wide_ff!J$5</f>
+        <v>2.9932675985723699E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f>[1]final_combined_8methods_wide_ff!A$7</f>
-        <v>fut_ESM1-2-LR_SSP370_constVolc</v>
+        <f>[2]final_combined_7methods_wide_ff!A$3</f>
+        <v>fut_ESM1-2-LR_SSP126_constVolc</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>ESM1-2-LR_SSP370_constVolc</v>
+        <f>RIGHT(A18,LEN(A18)-4)</f>
+        <v>ESM1-2-LR_SSP126_constVolc</v>
       </c>
       <c r="C18" s="3">
-        <f>[1]final_combined_8methods_wide_ff!C$7</f>
-        <v>0.60784617948213104</v>
+        <f>[2]final_combined_7methods_wide_ff!C$3</f>
+        <v>0.20598707423877799</v>
       </c>
       <c r="D18" s="3">
-        <f>[1]final_combined_8methods_wide_ff!D$7</f>
-        <v>0.89568249198837102</v>
+        <f>[2]final_combined_7methods_wide_ff!D$3</f>
+        <v>0.39125892210348001</v>
       </c>
       <c r="E18" s="3">
-        <f>[1]final_combined_8methods_wide_ff!E$7</f>
-        <v>0.99999998981716498</v>
-      </c>
-      <c r="F18" s="2">
-        <f>[1]final_combined_8methods_wide_ff!F$7</f>
-        <v>0.30125529255462702</v>
-      </c>
-      <c r="G18" s="2">
-        <f>[1]final_combined_8methods_wide_ff!G$7</f>
+        <f>[2]final_combined_7methods_wide_ff!E$3</f>
+        <v>0.75460221525915105</v>
+      </c>
+      <c r="F18" s="6">
+        <f>[2]final_combined_7methods_wide_ff!F$3</f>
+        <v>0.56475621844510304</v>
+      </c>
+      <c r="G18" s="6">
+        <f>[2]final_combined_7methods_wide_ff!G$3</f>
         <v>0</v>
       </c>
-      <c r="H18" s="2">
-        <f>[1]final_combined_8methods_wide_ff!H$7</f>
-        <v>1.06</v>
-      </c>
-      <c r="I18" s="1">
-        <f>[1]final_combined_8methods_wide_ff!I$7</f>
-        <v>3.1189349837246302E-2</v>
-      </c>
-      <c r="J18" s="1">
-        <f>[1]final_combined_8methods_wide_ff!J$7</f>
-        <v>2.8401842232407101E-2</v>
+      <c r="H18" s="6">
+        <f>[2]final_combined_7methods_wide_ff!H$3</f>
+        <v>1.42</v>
+      </c>
+      <c r="I18" s="5">
+        <f>[2]final_combined_7methods_wide_ff!I$3</f>
+        <v>3.52982195739854E-2</v>
+      </c>
+      <c r="J18" s="5">
+        <f>[2]final_combined_7methods_wide_ff!J$3</f>
+        <v>3.4435063627015101E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f>[1]final_combined_8methods_wide_ff!A$9</f>
-        <v>fut_NorESM_RCP45_Volc</v>
+        <f>[2]final_combined_7methods_wide_ff!A$11</f>
+        <v>fut_NorESM_RCP45_VolcConst</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>NorESM_RCP45_Volc</v>
+        <f>RIGHT(A19,LEN(A19)-4)</f>
+        <v>NorESM_RCP45_VolcConst</v>
       </c>
       <c r="C19" s="3">
-        <f>[1]final_combined_8methods_wide_ff!C$9</f>
-        <v>0.33924081974388598</v>
+        <f>[2]final_combined_7methods_wide_ff!C$11</f>
+        <v>0.54102601968391995</v>
       </c>
       <c r="D19" s="3">
-        <f>[1]final_combined_8methods_wide_ff!D$9</f>
-        <v>0.61175353856367198</v>
+        <f>[2]final_combined_7methods_wide_ff!D$11</f>
+        <v>0.86734724522561701</v>
       </c>
       <c r="E19" s="3">
-        <f>[1]final_combined_8methods_wide_ff!E$9</f>
-        <v>0.92475270821782396</v>
-      </c>
-      <c r="F19" s="2">
-        <f>[1]final_combined_8methods_wide_ff!F$9</f>
-        <v>0.63527200384498705</v>
-      </c>
-      <c r="G19" s="2">
-        <f>[1]final_combined_8methods_wide_ff!G$9</f>
+        <f>[2]final_combined_7methods_wide_ff!E$11</f>
+        <v>0.99999820550391105</v>
+      </c>
+      <c r="F19" s="6">
+        <f>[2]final_combined_7methods_wide_ff!F$11</f>
+        <v>0.588634202813348</v>
+      </c>
+      <c r="G19" s="6">
+        <f>[2]final_combined_7methods_wide_ff!G$11</f>
         <v>0</v>
       </c>
-      <c r="H19" s="2">
-        <f>[1]final_combined_8methods_wide_ff!H$9</f>
-        <v>1.06666666666666</v>
-      </c>
-      <c r="I19" s="1">
-        <f>[1]final_combined_8methods_wide_ff!I$9</f>
-        <v>4.5672518021823302E-2</v>
-      </c>
-      <c r="J19" s="1">
-        <f>[1]final_combined_8methods_wide_ff!J$9</f>
-        <v>4.7148170683740498E-2</v>
+      <c r="H19" s="6">
+        <f>[2]final_combined_7methods_wide_ff!H$11</f>
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
+        <f>[2]final_combined_7methods_wide_ff!I$11</f>
+        <v>2.9942905637516601E-2</v>
+      </c>
+      <c r="J19" s="5">
+        <f>[2]final_combined_7methods_wide_ff!J$11</f>
+        <v>3.0024013511340601E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f>[1]final_combined_8methods_wide_ff!A$11</f>
-        <v>fut_NorESM_RCP45_VolcConst</v>
+        <f>[2]final_combined_7methods_wide_ff!A$9</f>
+        <v>fut_NorESM_RCP45_Volc</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>NorESM_RCP45_VolcConst</v>
+        <f>RIGHT(A20,LEN(A20)-4)</f>
+        <v>NorESM_RCP45_Volc</v>
       </c>
       <c r="C20" s="3">
-        <f>[1]final_combined_8methods_wide_ff!C$11</f>
-        <v>0.582823059441401</v>
+        <f>[2]final_combined_7methods_wide_ff!C$9</f>
+        <v>0.29728047786762701</v>
       </c>
       <c r="D20" s="3">
-        <f>[1]final_combined_8methods_wide_ff!D$11</f>
-        <v>0.88205120151754801</v>
+        <f>[2]final_combined_7methods_wide_ff!D$9</f>
+        <v>0.54511819223838698</v>
       </c>
       <c r="E20" s="3">
-        <f>[1]final_combined_8methods_wide_ff!E$11</f>
-        <v>0.99999399718521598</v>
-      </c>
-      <c r="F20" s="2">
-        <f>[1]final_combined_8methods_wide_ff!F$11</f>
-        <v>0.42914306835327898</v>
-      </c>
-      <c r="G20" s="2">
-        <f>[1]final_combined_8methods_wide_ff!G$11</f>
+        <f>[2]final_combined_7methods_wide_ff!E$9</f>
+        <v>0.87959810607169198</v>
+      </c>
+      <c r="F20" s="6">
+        <f>[2]final_combined_7methods_wide_ff!F$9</f>
+        <v>0.75713434312233396</v>
+      </c>
+      <c r="G20" s="6">
+        <f>[2]final_combined_7methods_wide_ff!G$9</f>
         <v>0</v>
       </c>
-      <c r="H20" s="2">
-        <f>[1]final_combined_8methods_wide_ff!H$11</f>
-        <v>1.0166666666666599</v>
-      </c>
-      <c r="I20" s="1">
-        <f>[1]final_combined_8methods_wide_ff!I$11</f>
-        <v>2.69319364673281E-2</v>
-      </c>
-      <c r="J20" s="1">
-        <f>[1]final_combined_8methods_wide_ff!J$11</f>
-        <v>2.6904618104796E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="H20" s="6">
+        <f>[2]final_combined_7methods_wide_ff!H$9</f>
+        <v>1.11666666666666</v>
+      </c>
+      <c r="I20" s="5">
+        <f>[2]final_combined_7methods_wide_ff!I$9</f>
+        <v>4.9593159564462398E-2</v>
+      </c>
+      <c r="J20" s="5">
+        <f>[2]final_combined_7methods_wide_ff!J$9</f>
+        <v>5.1204322773566999E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C22" s="3" t="s">
@@ -1973,7 +1966,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f>[2]final_combined_16methods_wide_f!A$2</f>
+        <f>[1]final_combined_16methods_wide_f!A$2</f>
         <v>fut_ESM1-2-LR_SSP126_constVolc</v>
       </c>
       <c r="B23" t="str">
@@ -1981,41 +1974,41 @@
         <v>ESM1-2-LR_SSP126_constVolc</v>
       </c>
       <c r="C23" s="3">
-        <f>[2]final_combined_16methods_wide_f!C$2</f>
+        <f>[1]final_combined_16methods_wide_f!C$2</f>
         <v>0.23423231205582501</v>
       </c>
       <c r="D23" s="3">
-        <f>[2]final_combined_16methods_wide_f!D$2</f>
+        <f>[1]final_combined_16methods_wide_f!D$2</f>
         <v>0.44301513220746003</v>
       </c>
       <c r="E23" s="3">
-        <f>[2]final_combined_16methods_wide_f!E$2</f>
+        <f>[1]final_combined_16methods_wide_f!E$2</f>
         <v>0.80477747916472697</v>
       </c>
       <c r="F23" s="2">
-        <f>[2]final_combined_16methods_wide_f!F$2</f>
+        <f>[1]final_combined_16methods_wide_f!F$2</f>
         <v>0.46624181380279101</v>
       </c>
       <c r="G23" s="2">
-        <f>[2]final_combined_16methods_wide_f!G$2</f>
+        <f>[1]final_combined_16methods_wide_f!G$2</f>
         <v>0.49304442107483998</v>
       </c>
       <c r="H23" s="2">
-        <f>[2]final_combined_16methods_wide_f!H$2</f>
+        <f>[1]final_combined_16methods_wide_f!H$2</f>
         <v>1.22</v>
       </c>
       <c r="I23" s="1">
-        <f>[2]final_combined_16methods_wide_f!I$2</f>
+        <f>[1]final_combined_16methods_wide_f!I$2</f>
         <v>3.4209966316283001E-2</v>
       </c>
       <c r="J23" s="1">
-        <f>[2]final_combined_16methods_wide_f!J$2</f>
+        <f>[1]final_combined_16methods_wide_f!J$2</f>
         <v>3.3170670153985497E-2</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f>[2]final_combined_16methods_wide_f!A$4</f>
+        <f>[1]final_combined_16methods_wide_f!A$4</f>
         <v>fut_ESM1-2-LR_SSP245_constVolc</v>
       </c>
       <c r="B24" t="str">
@@ -2023,41 +2016,41 @@
         <v>ESM1-2-LR_SSP245_constVolc</v>
       </c>
       <c r="C24" s="3">
-        <f>[2]final_combined_16methods_wide_f!C$4</f>
+        <f>[1]final_combined_16methods_wide_f!C$4</f>
         <v>0.54526216461403398</v>
       </c>
       <c r="D24" s="3">
-        <f>[2]final_combined_16methods_wide_f!D$4</f>
+        <f>[1]final_combined_16methods_wide_f!D$4</f>
         <v>0.85151612528392695</v>
       </c>
       <c r="E24" s="3">
-        <f>[2]final_combined_16methods_wide_f!E$4</f>
+        <f>[1]final_combined_16methods_wide_f!E$4</f>
         <v>0.98769878415374102</v>
       </c>
       <c r="F24" s="2">
-        <f>[2]final_combined_16methods_wide_f!F$4</f>
+        <f>[1]final_combined_16methods_wide_f!F$4</f>
         <v>0.34391488294497302</v>
       </c>
       <c r="G24" s="2">
-        <f>[2]final_combined_16methods_wide_f!G$4</f>
+        <f>[1]final_combined_16methods_wide_f!G$4</f>
         <v>0.33005863001684399</v>
       </c>
       <c r="H24" s="2">
-        <f>[2]final_combined_16methods_wide_f!H$4</f>
+        <f>[1]final_combined_16methods_wide_f!H$4</f>
         <v>1.02</v>
       </c>
       <c r="I24" s="1">
-        <f>[2]final_combined_16methods_wide_f!I$4</f>
+        <f>[1]final_combined_16methods_wide_f!I$4</f>
         <v>3.1604406760897701E-2</v>
       </c>
       <c r="J24" s="1">
-        <f>[2]final_combined_16methods_wide_f!J$4</f>
+        <f>[1]final_combined_16methods_wide_f!J$4</f>
         <v>2.94731342330086E-2</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <f>[2]final_combined_16methods_wide_f!A$6</f>
+        <f>[1]final_combined_16methods_wide_f!A$6</f>
         <v>fut_ESM1-2-LR_SSP370_constVolc</v>
       </c>
       <c r="B25" t="str">
@@ -2065,41 +2058,41 @@
         <v>ESM1-2-LR_SSP370_constVolc</v>
       </c>
       <c r="C25" s="3">
-        <f>[2]final_combined_16methods_wide_f!C$6</f>
+        <f>[1]final_combined_16methods_wide_f!C$6</f>
         <v>0.58820103523420497</v>
       </c>
       <c r="D25" s="3">
-        <f>[2]final_combined_16methods_wide_f!D$6</f>
+        <f>[1]final_combined_16methods_wide_f!D$6</f>
         <v>0.882503084666731</v>
       </c>
       <c r="E25" s="3">
-        <f>[2]final_combined_16methods_wide_f!E$6</f>
+        <f>[1]final_combined_16methods_wide_f!E$6</f>
         <v>0.99999998110849297</v>
       </c>
       <c r="F25" s="2">
-        <f>[2]final_combined_16methods_wide_f!F$6</f>
+        <f>[1]final_combined_16methods_wide_f!F$6</f>
         <v>0.25605969664375</v>
       </c>
       <c r="G25" s="2">
-        <f>[2]final_combined_16methods_wide_f!G$6</f>
+        <f>[1]final_combined_16methods_wide_f!G$6</f>
         <v>0.18398203276660599</v>
       </c>
       <c r="H25" s="2">
-        <f>[2]final_combined_16methods_wide_f!H$6</f>
+        <f>[1]final_combined_16methods_wide_f!H$6</f>
         <v>1</v>
       </c>
       <c r="I25" s="1">
-        <f>[2]final_combined_16methods_wide_f!I$6</f>
+        <f>[1]final_combined_16methods_wide_f!I$6</f>
         <v>3.2646386575724898E-2</v>
       </c>
       <c r="J25" s="1">
-        <f>[2]final_combined_16methods_wide_f!J$6</f>
+        <f>[1]final_combined_16methods_wide_f!J$6</f>
         <v>2.8700340830130601E-2</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <f>[2]final_combined_16methods_wide_f!A$8</f>
+        <f>[1]final_combined_16methods_wide_f!A$8</f>
         <v>fut_NorESM_RCP45_Volc</v>
       </c>
       <c r="B26" t="str">
@@ -2107,41 +2100,41 @@
         <v>NorESM_RCP45_Volc</v>
       </c>
       <c r="C26" s="3">
-        <f>[2]final_combined_16methods_wide_f!C$8</f>
+        <f>[1]final_combined_16methods_wide_f!C$8</f>
         <v>0.31504677447179003</v>
       </c>
       <c r="D26" s="3">
-        <f>[2]final_combined_16methods_wide_f!D$8</f>
+        <f>[1]final_combined_16methods_wide_f!D$8</f>
         <v>0.57232123229446896</v>
       </c>
       <c r="E26" s="3">
-        <f>[2]final_combined_16methods_wide_f!E$8</f>
+        <f>[1]final_combined_16methods_wide_f!E$8</f>
         <v>0.89159107765915202</v>
       </c>
       <c r="F26" s="2">
-        <f>[2]final_combined_16methods_wide_f!F$8</f>
+        <f>[1]final_combined_16methods_wide_f!F$8</f>
         <v>0.65038981916972405</v>
       </c>
       <c r="G26" s="2">
-        <f>[2]final_combined_16methods_wide_f!G$8</f>
+        <f>[1]final_combined_16methods_wide_f!G$8</f>
         <v>0.69969231489820405</v>
       </c>
       <c r="H26" s="2">
-        <f>[2]final_combined_16methods_wide_f!H$8</f>
+        <f>[1]final_combined_16methods_wide_f!H$8</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="I26" s="1">
-        <f>[2]final_combined_16methods_wide_f!I$8</f>
+        <f>[1]final_combined_16methods_wide_f!I$8</f>
         <v>4.9608096699926101E-2</v>
       </c>
       <c r="J26" s="1">
-        <f>[2]final_combined_16methods_wide_f!J$8</f>
+        <f>[1]final_combined_16methods_wide_f!J$8</f>
         <v>5.1449692451564499E-2</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <f>[2]final_combined_16methods_wide_f!A$10</f>
+        <f>[1]final_combined_16methods_wide_f!A$10</f>
         <v>fut_NorESM_RCP45_VolcConst</v>
       </c>
       <c r="B27" t="str">
@@ -2149,35 +2142,35 @@
         <v>NorESM_RCP45_VolcConst</v>
       </c>
       <c r="C27" s="3">
-        <f>[2]final_combined_16methods_wide_f!C$10</f>
+        <f>[1]final_combined_16methods_wide_f!C$10</f>
         <v>0.60445409265483296</v>
       </c>
       <c r="D27" s="3">
-        <f>[2]final_combined_16methods_wide_f!D$10</f>
+        <f>[1]final_combined_16methods_wide_f!D$10</f>
         <v>0.91644379909259599</v>
       </c>
       <c r="E27" s="3">
-        <f>[2]final_combined_16methods_wide_f!E$10</f>
+        <f>[1]final_combined_16methods_wide_f!E$10</f>
         <v>0.99999999918240301</v>
       </c>
       <c r="F27" s="2">
-        <f>[2]final_combined_16methods_wide_f!F$10</f>
+        <f>[1]final_combined_16methods_wide_f!F$10</f>
         <v>0.39538783081048301</v>
       </c>
       <c r="G27" s="2">
-        <f>[2]final_combined_16methods_wide_f!G$10</f>
+        <f>[1]final_combined_16methods_wide_f!G$10</f>
         <v>0.42024078216599597</v>
       </c>
       <c r="H27" s="2">
-        <f>[2]final_combined_16methods_wide_f!H$10</f>
+        <f>[1]final_combined_16methods_wide_f!H$10</f>
         <v>1.0166666666666599</v>
       </c>
       <c r="I27" s="1">
-        <f>[2]final_combined_16methods_wide_f!I$10</f>
+        <f>[1]final_combined_16methods_wide_f!I$10</f>
         <v>2.8010350719259801E-2</v>
       </c>
       <c r="J27" s="1">
-        <f>[2]final_combined_16methods_wide_f!J$10</f>
+        <f>[1]final_combined_16methods_wide_f!J$10</f>
         <v>2.7966801098772701E-2</v>
       </c>
     </row>
@@ -2205,44 +2198,44 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
-        <f>A2</f>
-        <v>fut_ESM1-2-LR_SSP126_constVolc</v>
+        <f>A6</f>
+        <v>fut_ESM1-2-LR_SSP370_constVolc</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="0"/>
-        <v>ESM1-2-LR_SSP126_constVolc</v>
+        <f>RIGHT(A30,LEN(A30)-4)</f>
+        <v>ESM1-2-LR_SSP370_constVolc</v>
       </c>
       <c r="C30" s="3">
-        <f>C2</f>
-        <v>0.193323599140513</v>
+        <f>C6</f>
+        <v>0.64167468205339295</v>
       </c>
       <c r="D30" s="3">
-        <f>D2</f>
-        <v>0.380216728418869</v>
+        <f>D6</f>
+        <v>0.92134192098814205</v>
       </c>
       <c r="E30" s="3">
-        <f>E2</f>
-        <v>0.78584092298366603</v>
+        <f>E6</f>
+        <v>0.99999999992211497</v>
       </c>
       <c r="F30" s="2">
-        <f>F2</f>
-        <v>0.59962577107472603</v>
+        <f>F6</f>
+        <v>0.58257242065806303</v>
       </c>
       <c r="G30" s="2">
-        <f>G2</f>
-        <v>0.62717374477799903</v>
+        <f>G6</f>
+        <v>0.36471938323216702</v>
       </c>
       <c r="H30" s="2">
-        <f>H2</f>
-        <v>1.52</v>
+        <f>H6</f>
+        <v>1.06</v>
       </c>
       <c r="I30" s="1">
-        <f>I2</f>
-        <v>3.9122765985414802E-2</v>
+        <f>I6</f>
+        <v>3.9146185155741801E-2</v>
       </c>
       <c r="J30" s="1">
-        <f>J2</f>
-        <v>3.9793504476862397E-2</v>
+        <f>J6</f>
+        <v>2.9479803361305599E-2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -2255,173 +2248,168 @@
         <v>ESM1-2-LR_SSP245_constVolc</v>
       </c>
       <c r="C31" s="3">
-        <f>C4</f>
-        <v>0.53135273482905598</v>
+        <f t="shared" ref="C31:J31" si="1">C4</f>
+        <v>0.50974682042109598</v>
       </c>
       <c r="D31" s="3">
-        <f>D4</f>
-        <v>0.82636970138093202</v>
+        <f t="shared" si="1"/>
+        <v>0.80996193536411498</v>
       </c>
       <c r="E31" s="3">
-        <f>E4</f>
-        <v>0.99079631936799195</v>
+        <f t="shared" si="1"/>
+        <v>0.98746274665149802</v>
       </c>
       <c r="F31" s="2">
-        <f>F4</f>
-        <v>0.55943310164726401</v>
+        <f t="shared" si="1"/>
+        <v>0.56415571141182597</v>
       </c>
       <c r="G31" s="2">
-        <f>G4</f>
-        <v>0.58678766020784501</v>
+        <f t="shared" si="1"/>
+        <v>0.39092663554097901</v>
       </c>
       <c r="H31" s="2">
-        <f>H4</f>
+        <f t="shared" si="1"/>
         <v>1.02</v>
       </c>
       <c r="I31" s="1">
-        <f>I4</f>
-        <v>3.9053609917750497E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.9619484294593298E-2</v>
       </c>
       <c r="J31" s="1">
-        <f>J4</f>
-        <v>4.01043089335959E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.2487978546580497E-2</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <f>A6</f>
-        <v>fut_ESM1-2-LR_SSP370_constVolc</v>
+        <f>A2</f>
+        <v>fut_ESM1-2-LR_SSP126_constVolc</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>ESM1-2-LR_SSP370_constVolc</v>
+        <f>RIGHT(A32,LEN(A32)-4)</f>
+        <v>ESM1-2-LR_SSP126_constVolc</v>
       </c>
       <c r="C32" s="3">
-        <f>C6</f>
-        <v>0.576123416097439</v>
+        <f>C2</f>
+        <v>0.21161932405351599</v>
       </c>
       <c r="D32" s="3">
-        <f>D6</f>
-        <v>0.84515713805507198</v>
+        <f>D2</f>
+        <v>0.40396595365675098</v>
       </c>
       <c r="E32" s="3">
-        <f>E6</f>
-        <v>0.99999825056773195</v>
+        <f>E2</f>
+        <v>0.76865427585143098</v>
       </c>
       <c r="F32" s="2">
-        <f>F6</f>
-        <v>0.66091742730965497</v>
+        <f>F2</f>
+        <v>0.63734650833749396</v>
       </c>
       <c r="G32" s="2">
-        <f>G6</f>
-        <v>0.67416000173234703</v>
+        <f>G2</f>
+        <v>0.52549062434882099</v>
       </c>
       <c r="H32" s="2">
-        <f>H6</f>
-        <v>1.06</v>
+        <f>H2</f>
+        <v>1.54</v>
       </c>
       <c r="I32" s="1">
-        <f>I6</f>
-        <v>3.5884994681368902E-2</v>
+        <f>I2</f>
+        <v>4.14550484967314E-2</v>
       </c>
       <c r="J32" s="1">
-        <f>J6</f>
-        <v>3.5317593409777699E-2</v>
+        <f>J2</f>
+        <v>3.5818757452349699E-2</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
+        <f>A10</f>
+        <v>fut_NorESM_RCP45_VolcConst</v>
+      </c>
+      <c r="B33" t="str">
+        <f>RIGHT(A33,LEN(A33)-4)</f>
+        <v>NorESM_RCP45_VolcConst</v>
+      </c>
+      <c r="C33" s="3">
+        <f>C10</f>
+        <v>0.49934996162543499</v>
+      </c>
+      <c r="D33" s="3">
+        <f>D10</f>
+        <v>0.85184374092964499</v>
+      </c>
+      <c r="E33" s="3">
+        <f>E10</f>
+        <v>0.99999419553518598</v>
+      </c>
+      <c r="F33" s="2">
+        <f>F10</f>
+        <v>0.57230663609077204</v>
+      </c>
+      <c r="G33" s="2">
+        <f>G10</f>
+        <v>0.42470431846740098</v>
+      </c>
+      <c r="H33" s="2">
+        <f>H10</f>
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
+        <f>I10</f>
+        <v>2.9102690918756099E-2</v>
+      </c>
+      <c r="J33" s="1">
+        <f>J10</f>
+        <v>2.49146921749391E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="str">
         <f>A8</f>
         <v>fut_NorESM_RCP45_Volc</v>
       </c>
-      <c r="B33" t="str">
-        <f t="shared" si="0"/>
+      <c r="B34" t="str">
+        <f>RIGHT(A34,LEN(A34)-4)</f>
         <v>NorESM_RCP45_Volc</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C34" s="3">
         <f>C8</f>
-        <v>0.243835969387696</v>
-      </c>
-      <c r="D33" s="3">
+        <v>0.35316813126645102</v>
+      </c>
+      <c r="D34" s="3">
         <f>D8</f>
-        <v>0.47229445778025297</v>
-      </c>
-      <c r="E33" s="3">
+        <v>0.62991221212830595</v>
+      </c>
+      <c r="E34" s="3">
         <f>E8</f>
-        <v>0.88069455042945799</v>
-      </c>
-      <c r="F33" s="2">
+        <v>0.92104559023504595</v>
+      </c>
+      <c r="F34" s="2">
         <f>F8</f>
-        <v>0.78916143656328597</v>
-      </c>
-      <c r="G33" s="2">
+        <v>0.69470880820399195</v>
+      </c>
+      <c r="G34" s="2">
         <f>G8</f>
-        <v>0.88403148247910701</v>
-      </c>
-      <c r="H33" s="2">
+        <v>0.65259499157233103</v>
+      </c>
+      <c r="H34" s="2">
         <f>H8</f>
-        <v>1.06666666666666</v>
-      </c>
-      <c r="I33" s="1">
+        <v>1.11666666666666</v>
+      </c>
+      <c r="I34" s="1">
         <f>I8</f>
-        <v>6.6871679914844107E-2</v>
-      </c>
-      <c r="J33" s="1">
+        <v>5.9639432635513898E-2</v>
+      </c>
+      <c r="J34" s="1">
         <f>J8</f>
-        <v>7.3539784970054894E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" t="str">
-        <f>A10</f>
-        <v>fut_NorESM_RCP45_VolcConst</v>
-      </c>
-      <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>NorESM_RCP45_VolcConst</v>
-      </c>
-      <c r="C34" s="3">
-        <f>C10</f>
-        <v>0.319788720307984</v>
-      </c>
-      <c r="D34" s="3">
-        <f>D10</f>
-        <v>0.56955446780037</v>
-      </c>
-      <c r="E34" s="3">
-        <f>E10</f>
-        <v>0.96033614214204599</v>
-      </c>
-      <c r="F34" s="2">
-        <f>F10</f>
-        <v>0.71834740073190295</v>
-      </c>
-      <c r="G34" s="2">
-        <f>G10</f>
-        <v>0.77965408123227697</v>
-      </c>
-      <c r="H34" s="2">
-        <f>H10</f>
-        <v>1.0333333333333301</v>
-      </c>
-      <c r="I34" s="1">
-        <f>I10</f>
-        <v>4.9759412080330703E-2</v>
-      </c>
-      <c r="J34" s="1">
-        <f>J10</f>
-        <v>5.4092470432414802E-2</v>
+        <v>6.0089927606266198E-2</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C36" s="3" t="s">
@@ -2437,44 +2425,44 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <f>A3</f>
-        <v>fut_ESM1-2-LR_SSP126_constVolc</v>
+        <f>A7</f>
+        <v>fut_ESM1-2-LR_SSP370_constVolc</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
-        <v>ESM1-2-LR_SSP126_constVolc</v>
+        <v>ESM1-2-LR_SSP370_constVolc</v>
       </c>
       <c r="C37" s="3">
-        <f>C3</f>
-        <v>0.16500835590663099</v>
+        <f>C7</f>
+        <v>0.153679610448271</v>
       </c>
       <c r="D37" s="3">
-        <f>D3</f>
+        <f t="shared" ref="D37:J37" si="2">D3</f>
         <v>0.32052495709975298</v>
       </c>
       <c r="E37" s="3">
-        <f>E3</f>
+        <f t="shared" si="2"/>
         <v>0.67738862149364099</v>
       </c>
       <c r="F37" s="2">
-        <f>F3</f>
-        <v>0.71566361962981095</v>
+        <f t="shared" si="2"/>
+        <v>0.72312962730627905</v>
       </c>
       <c r="G37" s="2">
-        <f>G3</f>
-        <v>0.64250108122296601</v>
+        <f t="shared" si="2"/>
+        <v>0.65262018332211302</v>
       </c>
       <c r="H37" s="2">
-        <f>H3</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I37" s="1">
-        <f>I3</f>
-        <v>4.8024178941443202E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.7924826086253897E-2</v>
       </c>
       <c r="J37" s="1">
-        <f>J3</f>
-        <v>3.96099663956316E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.9585073275757901E-2</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -2487,165 +2475,166 @@
         <v>ESM1-2-LR_SSP245_constVolc</v>
       </c>
       <c r="C38" s="3">
-        <f>C5</f>
+        <f t="shared" ref="C38:J38" si="3">C5</f>
         <v>0.32272305160293702</v>
       </c>
       <c r="D38" s="3">
-        <f>D5</f>
+        <f t="shared" si="3"/>
         <v>0.60963225535908305</v>
       </c>
       <c r="E38" s="3">
-        <f>E5</f>
+        <f t="shared" si="3"/>
         <v>0.92550530731992098</v>
       </c>
       <c r="F38" s="2">
-        <f>F5</f>
-        <v>0.70551346522369296</v>
+        <f t="shared" si="3"/>
+        <v>0.71242307999963705</v>
       </c>
       <c r="G38" s="2">
-        <f>G5</f>
-        <v>0.60169079932651703</v>
+        <f t="shared" si="3"/>
+        <v>0.61013150635878699</v>
       </c>
       <c r="H38" s="2">
-        <f>H5</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I38" s="1">
-        <f>I5</f>
-        <v>5.1673175527618499E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.14577615073573E-2</v>
       </c>
       <c r="J38" s="1">
-        <f>J5</f>
-        <v>4.0134199225987002E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.9952145868938999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <f>A7</f>
-        <v>fut_ESM1-2-LR_SSP370_constVolc</v>
+        <f>A3</f>
+        <v>fut_ESM1-2-LR_SSP126_constVolc</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
-        <v>ESM1-2-LR_SSP370_constVolc</v>
+        <v>ESM1-2-LR_SSP126_constVolc</v>
       </c>
       <c r="C39" s="3">
-        <f>C7</f>
-        <v>0.153679610448271</v>
+        <f>C3</f>
+        <v>0.16500835590663099</v>
       </c>
       <c r="D39" s="3">
-        <f>D7</f>
+        <f t="shared" ref="D39:J39" si="4">D7</f>
         <v>0.34150036785639698</v>
       </c>
       <c r="E39" s="3">
-        <f>E7</f>
+        <f t="shared" si="4"/>
         <v>0.82410366011376901</v>
       </c>
       <c r="F39" s="2">
-        <f>F7</f>
-        <v>0.74998847518916401</v>
+        <f t="shared" si="4"/>
+        <v>0.75525220045584596</v>
       </c>
       <c r="G39" s="2">
-        <f>G7</f>
-        <v>0.64781887558101903</v>
+        <f t="shared" si="4"/>
+        <v>0.65528228338484396</v>
       </c>
       <c r="H39" s="2">
-        <f>H7</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I39" s="1">
-        <f>I7</f>
-        <v>6.8275797525348E-2</v>
+        <f t="shared" si="4"/>
+        <v>6.8233767139105395E-2</v>
       </c>
       <c r="J39" s="1">
-        <f>J7</f>
-        <v>5.7196022704550702E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.7310887082711301E-2</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
+        <f>A11</f>
+        <v>fut_NorESM_RCP45_VolcConst</v>
+      </c>
+      <c r="B40" t="str">
+        <f>RIGHT(A40,LEN(A40)-4)</f>
+        <v>NorESM_RCP45_VolcConst</v>
+      </c>
+      <c r="C40" s="3">
+        <f>C11</f>
+        <v>0.34149028921088098</v>
+      </c>
+      <c r="D40" s="3">
+        <f>D11</f>
+        <v>0.63497038219064394</v>
+      </c>
+      <c r="E40" s="3">
+        <f>E11</f>
+        <v>0.9887736478686</v>
+      </c>
+      <c r="F40" s="2">
+        <f>F11</f>
+        <v>0.73298331626506696</v>
+      </c>
+      <c r="G40" s="2">
+        <f>G11</f>
+        <v>0.67448595360081598</v>
+      </c>
+      <c r="H40" s="2">
+        <f>H11</f>
+        <v>1</v>
+      </c>
+      <c r="I40" s="1">
+        <f>I11</f>
+        <v>4.7962799242892498E-2</v>
+      </c>
+      <c r="J40" s="1">
+        <f>J11</f>
+        <v>4.2451274264061201E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="str">
         <f>A9</f>
         <v>fut_NorESM_RCP45_Volc</v>
       </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
+      <c r="B41" t="str">
+        <f>RIGHT(A41,LEN(A41)-4)</f>
         <v>NorESM_RCP45_Volc</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C41" s="3">
         <f>C9</f>
         <v>0.24172655046852501</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D41" s="3">
         <f>D9</f>
         <v>0.45951717349270299</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E41" s="3">
         <f>E9</f>
         <v>0.84197272967619696</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F41" s="2">
         <f>F9</f>
         <v>0.78885052339075301</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G41" s="2">
         <f>G9</f>
         <v>0.73038928215626897</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H41" s="2">
         <f>H9</f>
         <v>1.05</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I41" s="1">
         <f>I9</f>
         <v>6.00693062685295E-2</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J41" s="1">
         <f>J9</f>
         <v>5.5749640580537503E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" t="str">
-        <f>A11</f>
-        <v>fut_NorESM_RCP45_VolcConst</v>
-      </c>
-      <c r="B41" t="str">
-        <f t="shared" si="0"/>
-        <v>NorESM_RCP45_VolcConst</v>
-      </c>
-      <c r="C41" s="3">
-        <f>C11</f>
-        <v>0.34149028921088098</v>
-      </c>
-      <c r="D41" s="3">
-        <f>D11</f>
-        <v>0.63497038219064394</v>
-      </c>
-      <c r="E41" s="3">
-        <f>E11</f>
-        <v>0.9887736478686</v>
-      </c>
-      <c r="F41" s="2">
-        <f>F11</f>
-        <v>0.73298331626506696</v>
-      </c>
-      <c r="G41" s="2">
-        <f>G11</f>
-        <v>0.67448595360081598</v>
-      </c>
-      <c r="H41" s="2">
-        <f>H11</f>
-        <v>1</v>
-      </c>
-      <c r="I41" s="1">
-        <f>I11</f>
-        <v>4.7962799242892498E-2</v>
-      </c>
-      <c r="J41" s="1">
-        <f>J11</f>
-        <v>4.2451274264061201E-2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>